<commit_message>
Update Excel file with new user and employee data
- Add new user to Users worksheet for authentication
- Add new employee to Employee List worksheet for dropdown
- Sync local Excel changes with Streamlit Cloud deployment

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/TimeSheet Apps.xlsx
+++ b/TimeSheet Apps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c02271ef1bb6280a/timesheet_app_full_package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6E75BC3CDA63CABA861973FFF1A5261D0C677E92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04D08217-83DD-41F5-AA31-3FED3905C31D}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_6E75BC3CDA63CABA861973FFF1A5261D0C677E92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{804789BB-C923-57CF-AD9C-EB1A22466E98}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="15450" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeEntries" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Employee List with Graham ST HILAIRE
- Add missing employee: GRAHAM ST HILAIRE (15432I)
- Employee List now contains all 11 employees
- This will fix the missing Graham issue in Streamlit Cloud

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/TimeSheet Apps.xlsx
+++ b/TimeSheet Apps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c02271ef1bb6280a/timesheet_app_full_package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_6E75BC3CDA63CABA861973FFF1A5261D0C677E92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{804789BB-C923-57CF-AD9C-EB1A22466E98}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="11_6E75BC3CDA63CABA861973FFF1A5261D0C677E92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68645F0B-50FE-4ED1-8EAE-1402497CC7FF}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="15450" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="15450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeEntries" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="635">
   <si>
     <t>** Note: Please do not exceed 2000 rows of data.</t>
   </si>
@@ -1918,6 +1918,21 @@
   </si>
   <si>
     <t>nan</t>
+  </si>
+  <si>
+    <t>GRAHAM ST HILAIRE</t>
+  </si>
+  <si>
+    <t>15432I</t>
+  </si>
+  <si>
+    <t>Shawn Harcourt</t>
+  </si>
+  <si>
+    <t>SHarcourt@ptwenergy.com</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
@@ -2686,7 +2701,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2857,6 +2872,9 @@
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="center"/>
     </dxf>
@@ -2888,7 +2906,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="wholeTable" dxfId="25"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2958,8 +2976,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table6" displayName="Table6" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table6" displayName="Table6" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="User's Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email"/>
@@ -2972,15 +2990,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="EmployeeList" displayName="EmployeeList" ref="A1:J11" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:J11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J11">
-    <sortCondition ref="C1:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="EmployeeList" displayName="EmployeeList" ref="A1:J12" totalsRowShown="0" headerRowDxfId="24">
+  <autoFilter ref="A1:J12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J12">
+    <sortCondition ref="C1:C12"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Time Record Type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Person Number" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Employee Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Person Number" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Employee Name" dataDxfId="22"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Indirect / Direct" dataDxfId="21"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Override Trade Class"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Night Shift" dataDxfId="20"/>
@@ -2995,13 +3013,7 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="JobNumbers" displayName="JobNumbers" ref="A1:G44" totalsRowShown="0">
-  <autoFilter ref="A1:G44" xr:uid="{00000000-0009-0000-0100-000003000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G44" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="PROJECT NAME"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="AFE#"/>
@@ -9641,10 +9653,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9713,25 +9725,40 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>633</v>
+      </c>
+      <c r="D5" t="s">
+        <v>634</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{AEC6B1E7-6C2C-42E8-9A34-1595F8A8461F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9845,9 +9872,7 @@
       <c r="E4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>57</v>
-      </c>
+      <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -9873,9 +9898,7 @@
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="15">
-        <v>150</v>
-      </c>
+      <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15" t="b">
         <v>1</v>
@@ -9899,9 +9922,7 @@
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="15">
-        <v>150</v>
-      </c>
+      <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15" t="b">
         <v>1</v>
@@ -9925,9 +9946,7 @@
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="15">
-        <v>150</v>
-      </c>
+      <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15" t="b">
         <v>1</v>
@@ -9938,16 +9957,16 @@
         <v>45</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>64</v>
+        <v>631</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>630</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -9961,17 +9980,17 @@
       <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="20">
-        <v>17418</v>
+      <c r="B9" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -9986,23 +10005,23 @@
         <v>45</v>
       </c>
       <c r="B10" s="20">
-        <v>17163</v>
+        <v>17418</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -10010,22 +10029,46 @@
         <v>45</v>
       </c>
       <c r="B11" s="20">
-        <v>17446</v>
+        <v>17163</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="20">
+        <v>17446</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10042,7 +10085,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10079,7 +10122,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>78</v>
       </c>
@@ -10102,7 +10145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>78</v>
       </c>
@@ -10125,7 +10168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>78</v>
       </c>
@@ -10148,7 +10191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>78</v>
       </c>
@@ -10171,7 +10214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
@@ -10194,7 +10237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>78</v>
       </c>
@@ -10217,7 +10260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>78</v>
       </c>
@@ -10240,7 +10283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>78</v>
       </c>
@@ -10263,7 +10306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>78</v>
       </c>
@@ -10286,7 +10329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>78</v>
       </c>
@@ -10309,7 +10352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>78</v>
       </c>
@@ -10332,7 +10375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>78</v>
       </c>
@@ -10353,7 +10396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>78</v>
       </c>
@@ -10376,7 +10419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>112</v>
       </c>
@@ -10397,7 +10440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>112</v>
       </c>
@@ -10420,7 +10463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>78</v>
       </c>
@@ -10443,7 +10486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>78</v>
       </c>
@@ -10466,7 +10509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>78</v>
       </c>
@@ -10489,7 +10532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>78</v>
       </c>
@@ -10512,7 +10555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>112</v>
       </c>
@@ -10535,7 +10578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>112</v>
       </c>
@@ -10558,7 +10601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>112</v>
       </c>
@@ -10581,7 +10624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>112</v>
       </c>
@@ -10604,7 +10647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>78</v>
       </c>
@@ -10627,7 +10670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>78</v>
       </c>
@@ -10650,7 +10693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>78</v>
       </c>
@@ -10673,7 +10716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>112</v>
       </c>
@@ -10696,7 +10739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>112</v>
       </c>
@@ -10719,7 +10762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>78</v>
       </c>
@@ -10742,7 +10785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>78</v>
       </c>
@@ -10765,7 +10808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>78</v>
       </c>
@@ -10788,7 +10831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>78</v>
       </c>
@@ -10811,7 +10854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>78</v>
       </c>
@@ -10901,7 +10944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>112</v>
       </c>
@@ -10924,7 +10967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>112</v>
       </c>
@@ -10947,7 +10990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>112</v>
       </c>
@@ -10970,7 +11013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>112</v>
       </c>
@@ -11073,7 +11116,7 @@
   <dimension ref="A1:C323"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11167,7 +11210,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -14287,7 +14330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update cost code 00002-170-53 to Active=TRUE
- Project Management - Labour Expense Direct now set to TRUE
- Should appear in cost code dropdown after deployment

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/TimeSheet Apps.xlsx
+++ b/TimeSheet Apps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c02271ef1bb6280a/timesheet_app_full_package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_6E75BC3CDA63CABA861973FFF1A5261D0C677E92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68645F0B-50FE-4ED1-8EAE-1402497CC7FF}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_6E75BC3CDA63CABA861973FFF1A5261D0C677E92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F73D265-CD87-4F2A-891D-45C7349BF884}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="15450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="15450" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeEntries" sheetId="1" r:id="rId1"/>
@@ -9757,8 +9757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11115,8 +11115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C323"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11210,7 +11210,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update cost code 00002-170-53 back to Active=FALSE
- Project Management - Labour Expense Direct now set to FALSE
- Should be filtered OUT of cost code dropdown after deployment
- Testing auto-sync functionality

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/TimeSheet Apps.xlsx
+++ b/TimeSheet Apps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c02271ef1bb6280a/timesheet_app_full_package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_6E75BC3CDA63CABA861973FFF1A5261D0C677E92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F73D265-CD87-4F2A-891D-45C7349BF884}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_6E75BC3CDA63CABA861973FFF1A5261D0C677E92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A607B159-5324-4787-B728-0861CF18023E}"/>
   <bookViews>
     <workbookView xWindow="28830" yWindow="30" windowWidth="28770" windowHeight="15450" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11116,7 +11116,7 @@
   <dimension ref="A1:C323"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11210,7 +11210,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>